<commit_message>
updates on recent products from cookies
</commit_message>
<xml_diff>
--- a/relatedFiles/other files/final/products.xlsx
+++ b/relatedFiles/other files/final/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F605B94-0EEF-4144-8042-8B2BB92CF1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0173D04-C3DD-4E02-975B-0EC8811E9C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,9 +70,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>Total Product Units(Stock)</t>
-  </si>
-  <si>
     <t>Skin Tone</t>
   </si>
   <si>
@@ -535,6 +532,9 @@
   </si>
   <si>
     <t>normal-skin</t>
+  </si>
+  <si>
+    <t>Total Product Units</t>
   </si>
 </sst>
 </file>
@@ -883,13 +883,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="13.140625" style="1"/>
+    <col min="1" max="13" width="13.140625" style="1"/>
+    <col min="14" max="14" width="26.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="13.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -933,36 +935,36 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -971,7 +973,7 @@
         <v>46</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1">
         <v>30693</v>
@@ -980,33 +982,33 @@
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1015,7 +1017,7 @@
         <v>200</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M3" s="1">
         <v>30694</v>
@@ -1024,33 +1026,33 @@
         <v>10</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -1059,7 +1061,7 @@
         <v>145</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M4" s="1">
         <v>30695</v>
@@ -1068,33 +1070,33 @@
         <v>10</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -1103,7 +1105,7 @@
         <v>205</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M5" s="1">
         <v>30696</v>
@@ -1112,33 +1114,33 @@
         <v>10</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -1147,7 +1149,7 @@
         <v>130</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M6" s="1">
         <v>30697</v>
@@ -1156,33 +1158,33 @@
         <v>10</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -1191,7 +1193,7 @@
         <v>85</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M7" s="1">
         <v>30698</v>
@@ -1200,33 +1202,33 @@
         <v>10</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -1235,7 +1237,7 @@
         <v>45</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M8" s="1">
         <v>30699</v>
@@ -1244,33 +1246,33 @@
         <v>10</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -1279,7 +1281,7 @@
         <v>375</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M9" s="1">
         <v>30700</v>
@@ -1288,33 +1290,33 @@
         <v>10</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
@@ -1323,7 +1325,7 @@
         <v>365</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M10" s="1">
         <v>30701</v>
@@ -1332,33 +1334,33 @@
         <v>10</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1367,7 +1369,7 @@
         <v>375</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M11" s="1">
         <v>30702</v>
@@ -1376,33 +1378,33 @@
         <v>10</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -1411,7 +1413,7 @@
         <v>205</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M12" s="1">
         <v>30703</v>
@@ -1420,33 +1422,33 @@
         <v>10</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1455,7 +1457,7 @@
         <v>415</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M13" s="1">
         <v>30704</v>
@@ -1464,33 +1466,33 @@
         <v>10</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -1499,7 +1501,7 @@
         <v>135</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M14" s="1">
         <v>30705</v>
@@ -1508,33 +1510,33 @@
         <v>10</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -1543,7 +1545,7 @@
         <v>100</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M15" s="1">
         <v>30706</v>
@@ -1552,33 +1554,33 @@
         <v>10</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -1587,7 +1589,7 @@
         <v>300</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M16" s="1">
         <v>30707</v>
@@ -1596,33 +1598,33 @@
         <v>10</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -1631,7 +1633,7 @@
         <v>575</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M17" s="1">
         <v>30708</v>
@@ -1640,33 +1642,33 @@
         <v>10</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -1675,7 +1677,7 @@
         <v>130</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M18" s="1">
         <v>30709</v>
@@ -1684,33 +1686,33 @@
         <v>10</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -1719,7 +1721,7 @@
         <v>145</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M19" s="1">
         <v>30710</v>
@@ -1728,33 +1730,33 @@
         <v>10</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -1763,7 +1765,7 @@
         <v>350</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M20" s="1">
         <v>30711</v>
@@ -1772,33 +1774,33 @@
         <v>10</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -1807,7 +1809,7 @@
         <v>120</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M21" s="1">
         <v>30712</v>
@@ -1816,33 +1818,33 @@
         <v>10</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -1851,7 +1853,7 @@
         <v>210</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M22" s="1">
         <v>30713</v>
@@ -1860,33 +1862,33 @@
         <v>10</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -1895,7 +1897,7 @@
         <v>210</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M23" s="1">
         <v>30714</v>
@@ -1904,33 +1906,33 @@
         <v>10</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -1939,7 +1941,7 @@
         <v>50</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M24" s="1">
         <v>30715</v>
@@ -1948,33 +1950,33 @@
         <v>10</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -1983,7 +1985,7 @@
         <v>150</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M25" s="1">
         <v>30716</v>
@@ -1992,33 +1994,33 @@
         <v>10</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -2027,7 +2029,7 @@
         <v>210</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M26" s="1">
         <v>30717</v>
@@ -2036,33 +2038,33 @@
         <v>10</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -2071,7 +2073,7 @@
         <v>375</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M27" s="1">
         <v>30718</v>
@@ -2080,33 +2082,33 @@
         <v>10</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
@@ -2115,7 +2117,7 @@
         <v>215</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M28" s="1">
         <v>30719</v>
@@ -2124,33 +2126,33 @@
         <v>10</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" s="1">
         <v>0</v>
@@ -2159,7 +2161,7 @@
         <v>350</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M29" s="1">
         <v>30720</v>
@@ -2168,33 +2170,33 @@
         <v>10</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I30" s="1">
         <v>0</v>
@@ -2203,7 +2205,7 @@
         <v>200</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M30" s="1">
         <v>30721</v>
@@ -2212,33 +2214,33 @@
         <v>10</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -2247,7 +2249,7 @@
         <v>240</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M31" s="1">
         <v>30722</v>
@@ -2256,33 +2258,33 @@
         <v>10</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I32" s="1">
         <v>0</v>
@@ -2291,7 +2293,7 @@
         <v>205</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M32" s="1">
         <v>30723</v>
@@ -2300,33 +2302,33 @@
         <v>10</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -2335,7 +2337,7 @@
         <v>268</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M33" s="1">
         <v>30724</v>
@@ -2344,33 +2346,33 @@
         <v>10</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -2379,7 +2381,7 @@
         <v>268</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M34" s="1">
         <v>30725</v>
@@ -2388,33 +2390,33 @@
         <v>10</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -2423,7 +2425,7 @@
         <v>268</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M35" s="1">
         <v>30726</v>
@@ -2432,33 +2434,33 @@
         <v>10</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -2467,7 +2469,7 @@
         <v>268</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M36" s="1">
         <v>30727</v>
@@ -2476,7 +2478,7 @@
         <v>10</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>